<commit_message>
Site updated: 2019-02-04 13:17:33
</commit_message>
<xml_diff>
--- a/posts/成长记录/我的2019年目标跟踪记录/目标跟踪表.xlsx
+++ b/posts/成长记录/我的2019年目标跟踪记录/目标跟踪表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\Blog\source\_posts\成长记录\我的2019年目标跟踪记录\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8796DB81-6DCF-46A7-966A-5FBCFDD5B98B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD85BCED-48C9-4BC1-BC6C-A8D4D3B423AA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760" tabRatio="788" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="93">
   <si>
     <t>星期一</t>
   </si>
@@ -304,6 +304,322 @@
   </si>
   <si>
     <t>结束时间</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>如何阅读一本书</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://blog.ruanxinyu.cn/posts/%E8%AF%BB%E4%B9%A6%E7%AC%94%E8%AE%B0/%E5%A6%82%E4%BD%95%E9%98%85%E8%AF%BB%E4%B8%80%E6%9C%AC%E4%B9%A6/</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>写作是最好的自我投资</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://blog.ruanxinyu.cn/posts/%E8%AF%BB%E4%B9%A6%E7%AC%94%E8%AE%B0/%E5%86%99%E4%BD%9C%E6%98%AF%E6%9C%80%E5%A5%BD%E7%9A%84%E8%87%AA%E6%88%91%E6%8A%95%E8%B5%84/</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>区块链</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>定义未来金融与经济新格局</t>
+    </r>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://blog.ruanxinyu.cn/posts/%E8%AF%BB%E4%B9%A6%E7%AC%94%E8%AE%B0/%E5%8C%BA%E5%9D%97%E9%93%BE-%E5%AE%9A%E4%B9%89%E6%9C%AA%E6%9D%A5%E9%87%91%E8%9E%8D%E4%B8%8E%E7%BB%8F%E6%B5%8E%E6%96%B0%E6%A0%BC%E5%B1%80/</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://blog.ruanxinyu.cn/posts/%E8%AF%BB%E4%B9%A6%E7%AC%94%E8%AE%B0/%E7%9D%A1%E7%9C%A0%E9%9D%A9%E5%91%BD%EF%BC%9A%E5%A6%82%E4%BD%95%E8%AE%A9%E4%BD%A0%E7%9A%84%E7%9D%A1%E7%9C%A0%E6%9B%B4%E9%AB%98%E6%95%88/</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>睡眠革命：如何让你的睡眠更高效</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://blog.ruanxinyu.cn/posts/%E8%AF%BB%E4%B9%A6%E7%AC%94%E8%AE%B0/%E5%AD%90%E5%BC%B9%E7%AC%94%E8%AE%B0/</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>子弹笔记</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://blog.ruanxinyu.cn/posts/%E8%AF%BB%E4%B9%A6%E7%AC%94%E8%AE%B0/%E5%A6%82%E4%BD%95%E6%83%B3%E5%88%B0%E5%8F%88%E5%81%9A%E5%88%B0/</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>如何想到又做到</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://blog.ruanxinyu.cn/posts/%E8%AF%BB%E4%B9%A6%E7%AC%94%E8%AE%B0/%E4%B8%96%E7%95%8C%E5%9C%A8%E5%8F%98%E8%BD%AF/</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>世界在变软</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://blog.ruanxinyu.cn/posts/%E8%AF%BB%E4%B9%A6%E7%AC%94%E8%AE%B0/%E6%96%B0%E9%9B%B6%E5%94%AE%E6%97%B6%E4%BB%A3-%E6%9C%AA%E6%9D%A5%E9%9B%B6%E5%94%AE%E4%B8%9A%E7%9A%84%E6%96%B0%E4%B8%9A%E6%80%81/</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>新零售时代</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>未来零售业的新业态</t>
+    </r>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://blog.ruanxinyu.cn/posts/%E8%AF%BB%E4%B9%A6%E7%AC%94%E8%AE%B0/%E6%97%B6%E4%BB%A3%E4%B9%8B%E5%B7%85-%E4%BA%92%E8%81%94%E7%BD%91%E6%9E%84%E5%BB%BA%E6%96%B0%E7%BB%8F%E6%B5%8E/</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>时代之巅</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>互联网构建新经济</t>
+    </r>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>谁说你不能坚持</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>设计行为学</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>如何戒掉坏习惯</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>认知突围-做复杂时代的明白人</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>当前状态</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>已完成</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>笔记输出50%</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>快速工作法</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>待输出笔记</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>零秒工作法</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>已阅读</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>50%</t>
+    </r>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>已阅读</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>60%</t>
+    </r>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>思考快与慢</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>反本能-如何对抗你的习以为常</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>不抱怨的世界</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>学会学习-从认知自我到高效学习</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>练习的心态-如何培养耐心，专注和自律</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>关键</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>小时，快速学会任何技能</t>
+    </r>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>一分钟经理人</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>谁动了我的奶酪</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>习惯的力量</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>精进-如何成为一个很厉害的人</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>如何改变习惯-手把手教你用30天计划法改变95%的习惯</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
 </sst>
@@ -317,7 +633,7 @@
     <numFmt numFmtId="179" formatCode="0_);[Red]\(0\)"/>
     <numFmt numFmtId="182" formatCode="m&quot;月&quot;d&quot;日&quot;;@"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Trebuchet MS"/>
@@ -447,8 +763,30 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Trebuchet MS"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -510,6 +848,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -671,7 +1015,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
@@ -703,8 +1047,9 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -804,8 +1149,28 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="13" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="14">
     <cellStyle name="40% - 着色 1" xfId="1" builtinId="31" customBuiltin="1"/>
     <cellStyle name="备注" xfId="7" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="备注页眉" xfId="8" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
@@ -815,6 +1180,7 @@
     <cellStyle name="标题 3" xfId="11" builtinId="18" customBuiltin="1"/>
     <cellStyle name="标题 4" xfId="12" builtinId="19" customBuiltin="1"/>
     <cellStyle name="常规" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="超链接" xfId="13" builtinId="8"/>
     <cellStyle name="天" xfId="5" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
     <cellStyle name="天详细信息" xfId="6" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="着色 1" xfId="3" builtinId="29" customBuiltin="1"/>
@@ -2961,39 +3327,2223 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E4D57F-0E21-476E-8690-D5B02EB1AB90}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:I151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9" style="35"/>
+    <col min="2" max="2" width="50.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="11.875" style="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.875" customWidth="1"/>
+    <col min="8" max="8" width="149.25" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="37" t="s">
         <v>48</v>
       </c>
+      <c r="I1" s="38"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="39">
+        <v>1</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="38"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="39">
+        <v>2</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="I3" s="38"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="39">
+        <v>3</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" s="38"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="39">
+        <v>4</v>
+      </c>
+      <c r="B5" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="I5" s="38"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="39">
+        <v>5</v>
+      </c>
+      <c r="B6" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="38"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="39">
+        <v>6</v>
+      </c>
+      <c r="B7" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="I7" s="38"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="39">
+        <v>7</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="H8" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="I8" s="38"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="39">
+        <v>8</v>
+      </c>
+      <c r="B9" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="H9" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="I9" s="38"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="39">
+        <v>9</v>
+      </c>
+      <c r="B10" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" s="38"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="39">
+        <v>10</v>
+      </c>
+      <c r="B11" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="39">
+        <v>11</v>
+      </c>
+      <c r="B12" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="39">
+        <v>12</v>
+      </c>
+      <c r="B13" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="39">
+        <v>13</v>
+      </c>
+      <c r="B14" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="44">
+        <v>43497</v>
+      </c>
+      <c r="D14" s="44">
+        <v>43498</v>
+      </c>
+      <c r="E14" s="39">
+        <v>3</v>
+      </c>
+      <c r="F14" s="39"/>
+      <c r="G14" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="39">
+        <v>14</v>
+      </c>
+      <c r="B15" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="44">
+        <v>43498</v>
+      </c>
+      <c r="D15" s="44">
+        <v>43499</v>
+      </c>
+      <c r="E15" s="39">
+        <v>4.5</v>
+      </c>
+      <c r="F15" s="39"/>
+      <c r="G15" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="39">
+        <v>15</v>
+      </c>
+      <c r="B16" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="44">
+        <v>43499</v>
+      </c>
+      <c r="D16" s="44">
+        <v>43500</v>
+      </c>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="39">
+        <v>16</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="39">
+        <v>17</v>
+      </c>
+      <c r="B18" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="39">
+        <v>18</v>
+      </c>
+      <c r="B19" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="39">
+        <v>19</v>
+      </c>
+      <c r="B20" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="39">
+        <v>20</v>
+      </c>
+      <c r="B21" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="39">
+        <v>21</v>
+      </c>
+      <c r="B22" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="39">
+        <v>22</v>
+      </c>
+      <c r="B23" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="39">
+        <v>23</v>
+      </c>
+      <c r="B24" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="39">
+        <v>24</v>
+      </c>
+      <c r="B25" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="38"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="39">
+        <v>25</v>
+      </c>
+      <c r="B26" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" s="39"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="39">
+        <v>26</v>
+      </c>
+      <c r="B27" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="39">
+        <v>27</v>
+      </c>
+      <c r="B28" s="38"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="39">
+        <v>28</v>
+      </c>
+      <c r="B29" s="38"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="39">
+        <v>29</v>
+      </c>
+      <c r="B30" s="38"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="39">
+        <v>30</v>
+      </c>
+      <c r="B31" s="38"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="39">
+        <v>31</v>
+      </c>
+      <c r="B32" s="38"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="38"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="39">
+        <v>32</v>
+      </c>
+      <c r="B33" s="38"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="39"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="39">
+        <v>33</v>
+      </c>
+      <c r="B34" s="38"/>
+      <c r="C34" s="39"/>
+      <c r="D34" s="39"/>
+      <c r="E34" s="39"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="38"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="39">
+        <v>34</v>
+      </c>
+      <c r="B35" s="38"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="38"/>
+      <c r="I35" s="38"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="39">
+        <v>35</v>
+      </c>
+      <c r="B36" s="38"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="39"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="38"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="39">
+        <v>36</v>
+      </c>
+      <c r="B37" s="38"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="38"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="39">
+        <v>37</v>
+      </c>
+      <c r="B38" s="38"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="39"/>
+      <c r="E38" s="39"/>
+      <c r="F38" s="39"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="38"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="39">
+        <v>38</v>
+      </c>
+      <c r="B39" s="38"/>
+      <c r="C39" s="39"/>
+      <c r="D39" s="39"/>
+      <c r="E39" s="39"/>
+      <c r="F39" s="39"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="38"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="39">
+        <v>39</v>
+      </c>
+      <c r="B40" s="38"/>
+      <c r="C40" s="39"/>
+      <c r="D40" s="39"/>
+      <c r="E40" s="39"/>
+      <c r="F40" s="39"/>
+      <c r="G40" s="38"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="38"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="39">
+        <v>40</v>
+      </c>
+      <c r="B41" s="38"/>
+      <c r="C41" s="39"/>
+      <c r="D41" s="39"/>
+      <c r="E41" s="39"/>
+      <c r="F41" s="39"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="38"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="39">
+        <v>41</v>
+      </c>
+      <c r="B42" s="38"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="39"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="38"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="39">
+        <v>42</v>
+      </c>
+      <c r="B43" s="38"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="39"/>
+      <c r="E43" s="39"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="38"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="39">
+        <v>43</v>
+      </c>
+      <c r="B44" s="38"/>
+      <c r="C44" s="39"/>
+      <c r="D44" s="39"/>
+      <c r="E44" s="39"/>
+      <c r="F44" s="39"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="38"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="39">
+        <v>44</v>
+      </c>
+      <c r="B45" s="38"/>
+      <c r="C45" s="39"/>
+      <c r="D45" s="39"/>
+      <c r="E45" s="39"/>
+      <c r="F45" s="39"/>
+      <c r="G45" s="38"/>
+      <c r="H45" s="38"/>
+      <c r="I45" s="38"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" s="39">
+        <v>45</v>
+      </c>
+      <c r="B46" s="38"/>
+      <c r="C46" s="39"/>
+      <c r="D46" s="39"/>
+      <c r="E46" s="39"/>
+      <c r="F46" s="39"/>
+      <c r="G46" s="38"/>
+      <c r="H46" s="38"/>
+      <c r="I46" s="38"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" s="39">
+        <v>46</v>
+      </c>
+      <c r="B47" s="38"/>
+      <c r="C47" s="39"/>
+      <c r="D47" s="39"/>
+      <c r="E47" s="39"/>
+      <c r="F47" s="39"/>
+      <c r="G47" s="38"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="38"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" s="39">
+        <v>47</v>
+      </c>
+      <c r="B48" s="38"/>
+      <c r="C48" s="39"/>
+      <c r="D48" s="39"/>
+      <c r="E48" s="39"/>
+      <c r="F48" s="39"/>
+      <c r="G48" s="38"/>
+      <c r="H48" s="38"/>
+      <c r="I48" s="38"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="39">
+        <v>48</v>
+      </c>
+      <c r="B49" s="38"/>
+      <c r="C49" s="39"/>
+      <c r="D49" s="39"/>
+      <c r="E49" s="39"/>
+      <c r="F49" s="39"/>
+      <c r="G49" s="38"/>
+      <c r="H49" s="38"/>
+      <c r="I49" s="38"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="39">
+        <v>49</v>
+      </c>
+      <c r="B50" s="38"/>
+      <c r="C50" s="39"/>
+      <c r="D50" s="39"/>
+      <c r="E50" s="39"/>
+      <c r="F50" s="39"/>
+      <c r="G50" s="38"/>
+      <c r="H50" s="38"/>
+      <c r="I50" s="38"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="39">
+        <v>50</v>
+      </c>
+      <c r="B51" s="38"/>
+      <c r="C51" s="39"/>
+      <c r="D51" s="39"/>
+      <c r="E51" s="39"/>
+      <c r="F51" s="39"/>
+      <c r="G51" s="38"/>
+      <c r="H51" s="38"/>
+      <c r="I51" s="38"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" s="39">
+        <v>51</v>
+      </c>
+      <c r="B52" s="38"/>
+      <c r="C52" s="39"/>
+      <c r="D52" s="39"/>
+      <c r="E52" s="39"/>
+      <c r="F52" s="39"/>
+      <c r="G52" s="38"/>
+      <c r="H52" s="38"/>
+      <c r="I52" s="38"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" s="39">
+        <v>52</v>
+      </c>
+      <c r="B53" s="38"/>
+      <c r="C53" s="39"/>
+      <c r="D53" s="39"/>
+      <c r="E53" s="39"/>
+      <c r="F53" s="39"/>
+      <c r="G53" s="38"/>
+      <c r="H53" s="38"/>
+      <c r="I53" s="38"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" s="39">
+        <v>53</v>
+      </c>
+      <c r="B54" s="38"/>
+      <c r="C54" s="39"/>
+      <c r="D54" s="39"/>
+      <c r="E54" s="39"/>
+      <c r="F54" s="39"/>
+      <c r="G54" s="38"/>
+      <c r="H54" s="38"/>
+      <c r="I54" s="38"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" s="39">
+        <v>54</v>
+      </c>
+      <c r="B55" s="38"/>
+      <c r="C55" s="39"/>
+      <c r="D55" s="39"/>
+      <c r="E55" s="39"/>
+      <c r="F55" s="39"/>
+      <c r="G55" s="38"/>
+      <c r="H55" s="38"/>
+      <c r="I55" s="38"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" s="39">
+        <v>55</v>
+      </c>
+      <c r="B56" s="38"/>
+      <c r="C56" s="39"/>
+      <c r="D56" s="39"/>
+      <c r="E56" s="39"/>
+      <c r="F56" s="39"/>
+      <c r="G56" s="38"/>
+      <c r="H56" s="38"/>
+      <c r="I56" s="38"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" s="39">
+        <v>56</v>
+      </c>
+      <c r="B57" s="38"/>
+      <c r="C57" s="39"/>
+      <c r="D57" s="39"/>
+      <c r="E57" s="39"/>
+      <c r="F57" s="39"/>
+      <c r="G57" s="38"/>
+      <c r="H57" s="38"/>
+      <c r="I57" s="38"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" s="39">
+        <v>57</v>
+      </c>
+      <c r="B58" s="38"/>
+      <c r="C58" s="39"/>
+      <c r="D58" s="39"/>
+      <c r="E58" s="39"/>
+      <c r="F58" s="39"/>
+      <c r="G58" s="38"/>
+      <c r="H58" s="38"/>
+      <c r="I58" s="38"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" s="39">
+        <v>58</v>
+      </c>
+      <c r="B59" s="38"/>
+      <c r="C59" s="39"/>
+      <c r="D59" s="39"/>
+      <c r="E59" s="39"/>
+      <c r="F59" s="39"/>
+      <c r="G59" s="38"/>
+      <c r="H59" s="38"/>
+      <c r="I59" s="38"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="39">
+        <v>59</v>
+      </c>
+      <c r="B60" s="38"/>
+      <c r="C60" s="39"/>
+      <c r="D60" s="39"/>
+      <c r="E60" s="39"/>
+      <c r="F60" s="39"/>
+      <c r="G60" s="38"/>
+      <c r="H60" s="38"/>
+      <c r="I60" s="38"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61" s="39">
+        <v>60</v>
+      </c>
+      <c r="B61" s="38"/>
+      <c r="C61" s="39"/>
+      <c r="D61" s="39"/>
+      <c r="E61" s="39"/>
+      <c r="F61" s="39"/>
+      <c r="G61" s="38"/>
+      <c r="H61" s="38"/>
+      <c r="I61" s="38"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" s="39">
+        <v>61</v>
+      </c>
+      <c r="B62" s="38"/>
+      <c r="C62" s="39"/>
+      <c r="D62" s="39"/>
+      <c r="E62" s="39"/>
+      <c r="F62" s="39"/>
+      <c r="G62" s="38"/>
+      <c r="H62" s="38"/>
+      <c r="I62" s="38"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" s="39">
+        <v>62</v>
+      </c>
+      <c r="B63" s="38"/>
+      <c r="C63" s="39"/>
+      <c r="D63" s="39"/>
+      <c r="E63" s="39"/>
+      <c r="F63" s="39"/>
+      <c r="G63" s="38"/>
+      <c r="H63" s="38"/>
+      <c r="I63" s="38"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" s="39">
+        <v>63</v>
+      </c>
+      <c r="B64" s="38"/>
+      <c r="C64" s="39"/>
+      <c r="D64" s="39"/>
+      <c r="E64" s="39"/>
+      <c r="F64" s="39"/>
+      <c r="G64" s="38"/>
+      <c r="H64" s="38"/>
+      <c r="I64" s="38"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65" s="39">
+        <v>64</v>
+      </c>
+      <c r="B65" s="38"/>
+      <c r="C65" s="39"/>
+      <c r="D65" s="39"/>
+      <c r="E65" s="39"/>
+      <c r="F65" s="39"/>
+      <c r="G65" s="38"/>
+      <c r="H65" s="38"/>
+      <c r="I65" s="38"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66" s="39">
+        <v>65</v>
+      </c>
+      <c r="B66" s="38"/>
+      <c r="C66" s="39"/>
+      <c r="D66" s="39"/>
+      <c r="E66" s="39"/>
+      <c r="F66" s="39"/>
+      <c r="G66" s="38"/>
+      <c r="H66" s="38"/>
+      <c r="I66" s="38"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A67" s="39">
+        <v>66</v>
+      </c>
+      <c r="B67" s="38"/>
+      <c r="C67" s="39"/>
+      <c r="D67" s="39"/>
+      <c r="E67" s="39"/>
+      <c r="F67" s="39"/>
+      <c r="G67" s="38"/>
+      <c r="H67" s="38"/>
+      <c r="I67" s="38"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A68" s="39">
+        <v>67</v>
+      </c>
+      <c r="B68" s="38"/>
+      <c r="C68" s="39"/>
+      <c r="D68" s="39"/>
+      <c r="E68" s="39"/>
+      <c r="F68" s="39"/>
+      <c r="G68" s="38"/>
+      <c r="H68" s="38"/>
+      <c r="I68" s="38"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A69" s="39">
+        <v>68</v>
+      </c>
+      <c r="B69" s="38"/>
+      <c r="C69" s="39"/>
+      <c r="D69" s="39"/>
+      <c r="E69" s="39"/>
+      <c r="F69" s="39"/>
+      <c r="G69" s="38"/>
+      <c r="H69" s="38"/>
+      <c r="I69" s="38"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A70" s="39">
+        <v>69</v>
+      </c>
+      <c r="B70" s="38"/>
+      <c r="C70" s="39"/>
+      <c r="D70" s="39"/>
+      <c r="E70" s="39"/>
+      <c r="F70" s="39"/>
+      <c r="G70" s="38"/>
+      <c r="H70" s="38"/>
+      <c r="I70" s="38"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A71" s="39">
+        <v>70</v>
+      </c>
+      <c r="B71" s="38"/>
+      <c r="C71" s="39"/>
+      <c r="D71" s="39"/>
+      <c r="E71" s="39"/>
+      <c r="F71" s="39"/>
+      <c r="G71" s="38"/>
+      <c r="H71" s="38"/>
+      <c r="I71" s="38"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A72" s="39">
+        <v>71</v>
+      </c>
+      <c r="B72" s="38"/>
+      <c r="C72" s="39"/>
+      <c r="D72" s="39"/>
+      <c r="E72" s="39"/>
+      <c r="F72" s="39"/>
+      <c r="G72" s="38"/>
+      <c r="H72" s="38"/>
+      <c r="I72" s="38"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A73" s="39">
+        <v>72</v>
+      </c>
+      <c r="B73" s="38"/>
+      <c r="C73" s="39"/>
+      <c r="D73" s="39"/>
+      <c r="E73" s="39"/>
+      <c r="F73" s="39"/>
+      <c r="G73" s="38"/>
+      <c r="H73" s="38"/>
+      <c r="I73" s="38"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A74" s="39">
+        <v>73</v>
+      </c>
+      <c r="B74" s="38"/>
+      <c r="C74" s="39"/>
+      <c r="D74" s="39"/>
+      <c r="E74" s="39"/>
+      <c r="F74" s="39"/>
+      <c r="G74" s="38"/>
+      <c r="H74" s="38"/>
+      <c r="I74" s="38"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A75" s="39">
+        <v>74</v>
+      </c>
+      <c r="B75" s="38"/>
+      <c r="C75" s="39"/>
+      <c r="D75" s="39"/>
+      <c r="E75" s="39"/>
+      <c r="F75" s="39"/>
+      <c r="G75" s="38"/>
+      <c r="H75" s="38"/>
+      <c r="I75" s="38"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A76" s="39">
+        <v>75</v>
+      </c>
+      <c r="B76" s="38"/>
+      <c r="C76" s="39"/>
+      <c r="D76" s="39"/>
+      <c r="E76" s="39"/>
+      <c r="F76" s="39"/>
+      <c r="G76" s="38"/>
+      <c r="H76" s="38"/>
+      <c r="I76" s="38"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A77" s="39">
+        <v>76</v>
+      </c>
+      <c r="B77" s="38"/>
+      <c r="C77" s="39"/>
+      <c r="D77" s="39"/>
+      <c r="E77" s="39"/>
+      <c r="F77" s="39"/>
+      <c r="G77" s="38"/>
+      <c r="H77" s="38"/>
+      <c r="I77" s="38"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A78" s="39">
+        <v>77</v>
+      </c>
+      <c r="B78" s="38"/>
+      <c r="C78" s="39"/>
+      <c r="D78" s="39"/>
+      <c r="E78" s="39"/>
+      <c r="F78" s="39"/>
+      <c r="G78" s="38"/>
+      <c r="H78" s="38"/>
+      <c r="I78" s="38"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A79" s="39">
+        <v>78</v>
+      </c>
+      <c r="B79" s="38"/>
+      <c r="C79" s="39"/>
+      <c r="D79" s="39"/>
+      <c r="E79" s="39"/>
+      <c r="F79" s="39"/>
+      <c r="G79" s="38"/>
+      <c r="H79" s="38"/>
+      <c r="I79" s="38"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A80" s="39">
+        <v>79</v>
+      </c>
+      <c r="B80" s="38"/>
+      <c r="C80" s="39"/>
+      <c r="D80" s="39"/>
+      <c r="E80" s="39"/>
+      <c r="F80" s="39"/>
+      <c r="G80" s="38"/>
+      <c r="H80" s="38"/>
+      <c r="I80" s="38"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A81" s="39">
+        <v>80</v>
+      </c>
+      <c r="B81" s="38"/>
+      <c r="C81" s="39"/>
+      <c r="D81" s="39"/>
+      <c r="E81" s="39"/>
+      <c r="F81" s="39"/>
+      <c r="G81" s="38"/>
+      <c r="H81" s="38"/>
+      <c r="I81" s="38"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A82" s="39">
+        <v>81</v>
+      </c>
+      <c r="B82" s="38"/>
+      <c r="C82" s="39"/>
+      <c r="D82" s="39"/>
+      <c r="E82" s="39"/>
+      <c r="F82" s="39"/>
+      <c r="G82" s="38"/>
+      <c r="H82" s="38"/>
+      <c r="I82" s="38"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A83" s="39">
+        <v>82</v>
+      </c>
+      <c r="B83" s="38"/>
+      <c r="C83" s="39"/>
+      <c r="D83" s="39"/>
+      <c r="E83" s="39"/>
+      <c r="F83" s="39"/>
+      <c r="G83" s="38"/>
+      <c r="H83" s="38"/>
+      <c r="I83" s="38"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A84" s="39">
+        <v>83</v>
+      </c>
+      <c r="B84" s="38"/>
+      <c r="C84" s="39"/>
+      <c r="D84" s="39"/>
+      <c r="E84" s="39"/>
+      <c r="F84" s="39"/>
+      <c r="G84" s="38"/>
+      <c r="H84" s="38"/>
+      <c r="I84" s="38"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A85" s="39">
+        <v>84</v>
+      </c>
+      <c r="B85" s="38"/>
+      <c r="C85" s="39"/>
+      <c r="D85" s="39"/>
+      <c r="E85" s="39"/>
+      <c r="F85" s="39"/>
+      <c r="G85" s="38"/>
+      <c r="H85" s="38"/>
+      <c r="I85" s="38"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A86" s="39">
+        <v>85</v>
+      </c>
+      <c r="B86" s="38"/>
+      <c r="C86" s="39"/>
+      <c r="D86" s="39"/>
+      <c r="E86" s="39"/>
+      <c r="F86" s="39"/>
+      <c r="G86" s="38"/>
+      <c r="H86" s="38"/>
+      <c r="I86" s="38"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A87" s="39">
+        <v>86</v>
+      </c>
+      <c r="B87" s="38"/>
+      <c r="C87" s="39"/>
+      <c r="D87" s="39"/>
+      <c r="E87" s="39"/>
+      <c r="F87" s="39"/>
+      <c r="G87" s="38"/>
+      <c r="H87" s="38"/>
+      <c r="I87" s="38"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A88" s="39">
+        <v>87</v>
+      </c>
+      <c r="B88" s="38"/>
+      <c r="C88" s="39"/>
+      <c r="D88" s="39"/>
+      <c r="E88" s="39"/>
+      <c r="F88" s="39"/>
+      <c r="G88" s="38"/>
+      <c r="H88" s="38"/>
+      <c r="I88" s="38"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A89" s="39">
+        <v>88</v>
+      </c>
+      <c r="B89" s="38"/>
+      <c r="C89" s="39"/>
+      <c r="D89" s="39"/>
+      <c r="E89" s="39"/>
+      <c r="F89" s="39"/>
+      <c r="G89" s="38"/>
+      <c r="H89" s="38"/>
+      <c r="I89" s="38"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A90" s="39">
+        <v>89</v>
+      </c>
+      <c r="B90" s="38"/>
+      <c r="C90" s="39"/>
+      <c r="D90" s="39"/>
+      <c r="E90" s="39"/>
+      <c r="F90" s="39"/>
+      <c r="G90" s="38"/>
+      <c r="H90" s="38"/>
+      <c r="I90" s="38"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A91" s="39">
+        <v>90</v>
+      </c>
+      <c r="B91" s="38"/>
+      <c r="C91" s="39"/>
+      <c r="D91" s="39"/>
+      <c r="E91" s="39"/>
+      <c r="F91" s="39"/>
+      <c r="G91" s="38"/>
+      <c r="H91" s="38"/>
+      <c r="I91" s="38"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A92" s="39">
+        <v>91</v>
+      </c>
+      <c r="B92" s="38"/>
+      <c r="C92" s="39"/>
+      <c r="D92" s="39"/>
+      <c r="E92" s="39"/>
+      <c r="F92" s="39"/>
+      <c r="G92" s="38"/>
+      <c r="H92" s="38"/>
+      <c r="I92" s="38"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A93" s="39">
+        <v>92</v>
+      </c>
+      <c r="B93" s="38"/>
+      <c r="C93" s="39"/>
+      <c r="D93" s="39"/>
+      <c r="E93" s="39"/>
+      <c r="F93" s="39"/>
+      <c r="G93" s="38"/>
+      <c r="H93" s="38"/>
+      <c r="I93" s="38"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A94" s="39">
+        <v>93</v>
+      </c>
+      <c r="B94" s="38"/>
+      <c r="C94" s="39"/>
+      <c r="D94" s="39"/>
+      <c r="E94" s="39"/>
+      <c r="F94" s="39"/>
+      <c r="G94" s="38"/>
+      <c r="H94" s="38"/>
+      <c r="I94" s="38"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A95" s="39">
+        <v>94</v>
+      </c>
+      <c r="B95" s="38"/>
+      <c r="C95" s="39"/>
+      <c r="D95" s="39"/>
+      <c r="E95" s="39"/>
+      <c r="F95" s="39"/>
+      <c r="G95" s="38"/>
+      <c r="H95" s="38"/>
+      <c r="I95" s="38"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A96" s="39">
+        <v>95</v>
+      </c>
+      <c r="B96" s="38"/>
+      <c r="C96" s="39"/>
+      <c r="D96" s="39"/>
+      <c r="E96" s="39"/>
+      <c r="F96" s="39"/>
+      <c r="G96" s="38"/>
+      <c r="H96" s="38"/>
+      <c r="I96" s="38"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A97" s="39">
+        <v>96</v>
+      </c>
+      <c r="B97" s="38"/>
+      <c r="C97" s="39"/>
+      <c r="D97" s="39"/>
+      <c r="E97" s="39"/>
+      <c r="F97" s="39"/>
+      <c r="G97" s="38"/>
+      <c r="H97" s="38"/>
+      <c r="I97" s="38"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A98" s="39">
+        <v>97</v>
+      </c>
+      <c r="B98" s="38"/>
+      <c r="C98" s="39"/>
+      <c r="D98" s="39"/>
+      <c r="E98" s="39"/>
+      <c r="F98" s="39"/>
+      <c r="G98" s="38"/>
+      <c r="H98" s="38"/>
+      <c r="I98" s="38"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A99" s="39">
+        <v>98</v>
+      </c>
+      <c r="B99" s="38"/>
+      <c r="C99" s="39"/>
+      <c r="D99" s="39"/>
+      <c r="E99" s="39"/>
+      <c r="F99" s="39"/>
+      <c r="G99" s="38"/>
+      <c r="H99" s="38"/>
+      <c r="I99" s="38"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A100" s="39">
+        <v>99</v>
+      </c>
+      <c r="B100" s="38"/>
+      <c r="C100" s="39"/>
+      <c r="D100" s="39"/>
+      <c r="E100" s="39"/>
+      <c r="F100" s="39"/>
+      <c r="G100" s="38"/>
+      <c r="H100" s="38"/>
+      <c r="I100" s="38"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A101" s="39">
+        <v>100</v>
+      </c>
+      <c r="B101" s="38"/>
+      <c r="C101" s="39"/>
+      <c r="D101" s="39"/>
+      <c r="E101" s="39"/>
+      <c r="F101" s="39"/>
+      <c r="G101" s="38"/>
+      <c r="H101" s="38"/>
+      <c r="I101" s="38"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A102" s="39">
+        <v>101</v>
+      </c>
+      <c r="B102" s="38"/>
+      <c r="C102" s="39"/>
+      <c r="D102" s="39"/>
+      <c r="E102" s="39"/>
+      <c r="F102" s="39"/>
+      <c r="G102" s="38"/>
+      <c r="H102" s="38"/>
+      <c r="I102" s="38"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A103" s="39">
+        <v>102</v>
+      </c>
+      <c r="B103" s="38"/>
+      <c r="C103" s="39"/>
+      <c r="D103" s="39"/>
+      <c r="E103" s="39"/>
+      <c r="F103" s="39"/>
+      <c r="G103" s="38"/>
+      <c r="H103" s="38"/>
+      <c r="I103" s="38"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A104" s="39">
+        <v>103</v>
+      </c>
+      <c r="B104" s="38"/>
+      <c r="C104" s="39"/>
+      <c r="D104" s="39"/>
+      <c r="E104" s="39"/>
+      <c r="F104" s="39"/>
+      <c r="G104" s="38"/>
+      <c r="H104" s="38"/>
+      <c r="I104" s="38"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A105" s="39">
+        <v>104</v>
+      </c>
+      <c r="B105" s="38"/>
+      <c r="C105" s="39"/>
+      <c r="D105" s="39"/>
+      <c r="E105" s="39"/>
+      <c r="F105" s="39"/>
+      <c r="G105" s="38"/>
+      <c r="H105" s="38"/>
+      <c r="I105" s="38"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A106" s="39">
+        <v>105</v>
+      </c>
+      <c r="B106" s="38"/>
+      <c r="C106" s="39"/>
+      <c r="D106" s="39"/>
+      <c r="E106" s="39"/>
+      <c r="F106" s="39"/>
+      <c r="G106" s="38"/>
+      <c r="H106" s="38"/>
+      <c r="I106" s="38"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A107" s="39">
+        <v>106</v>
+      </c>
+      <c r="B107" s="38"/>
+      <c r="C107" s="39"/>
+      <c r="D107" s="39"/>
+      <c r="E107" s="39"/>
+      <c r="F107" s="39"/>
+      <c r="G107" s="38"/>
+      <c r="H107" s="38"/>
+      <c r="I107" s="38"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A108" s="39">
+        <v>107</v>
+      </c>
+      <c r="B108" s="38"/>
+      <c r="C108" s="39"/>
+      <c r="D108" s="39"/>
+      <c r="E108" s="39"/>
+      <c r="F108" s="39"/>
+      <c r="G108" s="38"/>
+      <c r="H108" s="38"/>
+      <c r="I108" s="38"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A109" s="39">
+        <v>108</v>
+      </c>
+      <c r="B109" s="38"/>
+      <c r="C109" s="39"/>
+      <c r="D109" s="39"/>
+      <c r="E109" s="39"/>
+      <c r="F109" s="39"/>
+      <c r="G109" s="38"/>
+      <c r="H109" s="38"/>
+      <c r="I109" s="38"/>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A110" s="39">
+        <v>109</v>
+      </c>
+      <c r="B110" s="38"/>
+      <c r="C110" s="39"/>
+      <c r="D110" s="39"/>
+      <c r="E110" s="39"/>
+      <c r="F110" s="39"/>
+      <c r="G110" s="38"/>
+      <c r="H110" s="38"/>
+      <c r="I110" s="38"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A111" s="39">
+        <v>110</v>
+      </c>
+      <c r="B111" s="38"/>
+      <c r="C111" s="39"/>
+      <c r="D111" s="39"/>
+      <c r="E111" s="39"/>
+      <c r="F111" s="39"/>
+      <c r="G111" s="38"/>
+      <c r="H111" s="38"/>
+      <c r="I111" s="38"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A112" s="39">
+        <v>111</v>
+      </c>
+      <c r="B112" s="38"/>
+      <c r="C112" s="39"/>
+      <c r="D112" s="39"/>
+      <c r="E112" s="39"/>
+      <c r="F112" s="39"/>
+      <c r="G112" s="38"/>
+      <c r="H112" s="38"/>
+      <c r="I112" s="38"/>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A113" s="39">
+        <v>112</v>
+      </c>
+      <c r="B113" s="38"/>
+      <c r="C113" s="39"/>
+      <c r="D113" s="39"/>
+      <c r="E113" s="39"/>
+      <c r="F113" s="39"/>
+      <c r="G113" s="38"/>
+      <c r="H113" s="38"/>
+      <c r="I113" s="38"/>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A114" s="39">
+        <v>113</v>
+      </c>
+      <c r="B114" s="38"/>
+      <c r="C114" s="39"/>
+      <c r="D114" s="39"/>
+      <c r="E114" s="39"/>
+      <c r="F114" s="39"/>
+      <c r="G114" s="38"/>
+      <c r="H114" s="38"/>
+      <c r="I114" s="38"/>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A115" s="39">
+        <v>114</v>
+      </c>
+      <c r="B115" s="38"/>
+      <c r="C115" s="39"/>
+      <c r="D115" s="39"/>
+      <c r="E115" s="39"/>
+      <c r="F115" s="39"/>
+      <c r="G115" s="38"/>
+      <c r="H115" s="38"/>
+      <c r="I115" s="38"/>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A116" s="39">
+        <v>115</v>
+      </c>
+      <c r="B116" s="38"/>
+      <c r="C116" s="39"/>
+      <c r="D116" s="39"/>
+      <c r="E116" s="39"/>
+      <c r="F116" s="39"/>
+      <c r="G116" s="38"/>
+      <c r="H116" s="38"/>
+      <c r="I116" s="38"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A117" s="39">
+        <v>116</v>
+      </c>
+      <c r="B117" s="38"/>
+      <c r="C117" s="39"/>
+      <c r="D117" s="39"/>
+      <c r="E117" s="39"/>
+      <c r="F117" s="39"/>
+      <c r="G117" s="38"/>
+      <c r="H117" s="38"/>
+      <c r="I117" s="38"/>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A118" s="39">
+        <v>117</v>
+      </c>
+      <c r="B118" s="38"/>
+      <c r="C118" s="39"/>
+      <c r="D118" s="39"/>
+      <c r="E118" s="39"/>
+      <c r="F118" s="39"/>
+      <c r="G118" s="38"/>
+      <c r="H118" s="38"/>
+      <c r="I118" s="38"/>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A119" s="39">
+        <v>118</v>
+      </c>
+      <c r="B119" s="38"/>
+      <c r="C119" s="39"/>
+      <c r="D119" s="39"/>
+      <c r="E119" s="39"/>
+      <c r="F119" s="39"/>
+      <c r="G119" s="38"/>
+      <c r="H119" s="38"/>
+      <c r="I119" s="38"/>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A120" s="39">
+        <v>119</v>
+      </c>
+      <c r="B120" s="38"/>
+      <c r="C120" s="39"/>
+      <c r="D120" s="39"/>
+      <c r="E120" s="39"/>
+      <c r="F120" s="39"/>
+      <c r="G120" s="38"/>
+      <c r="H120" s="38"/>
+      <c r="I120" s="38"/>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A121" s="39">
+        <v>120</v>
+      </c>
+      <c r="B121" s="38"/>
+      <c r="C121" s="39"/>
+      <c r="D121" s="39"/>
+      <c r="E121" s="39"/>
+      <c r="F121" s="39"/>
+      <c r="G121" s="38"/>
+      <c r="H121" s="38"/>
+      <c r="I121" s="38"/>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A122" s="39">
+        <v>121</v>
+      </c>
+      <c r="B122" s="38"/>
+      <c r="C122" s="39"/>
+      <c r="D122" s="39"/>
+      <c r="E122" s="39"/>
+      <c r="F122" s="39"/>
+      <c r="G122" s="38"/>
+      <c r="H122" s="38"/>
+      <c r="I122" s="38"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A123" s="39">
+        <v>122</v>
+      </c>
+      <c r="B123" s="38"/>
+      <c r="C123" s="39"/>
+      <c r="D123" s="39"/>
+      <c r="E123" s="39"/>
+      <c r="F123" s="39"/>
+      <c r="G123" s="38"/>
+      <c r="H123" s="38"/>
+      <c r="I123" s="38"/>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A124" s="39">
+        <v>123</v>
+      </c>
+      <c r="B124" s="38"/>
+      <c r="C124" s="39"/>
+      <c r="D124" s="39"/>
+      <c r="E124" s="39"/>
+      <c r="F124" s="39"/>
+      <c r="G124" s="38"/>
+      <c r="H124" s="38"/>
+      <c r="I124" s="38"/>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A125" s="39">
+        <v>124</v>
+      </c>
+      <c r="B125" s="38"/>
+      <c r="C125" s="39"/>
+      <c r="D125" s="39"/>
+      <c r="E125" s="39"/>
+      <c r="F125" s="39"/>
+      <c r="G125" s="38"/>
+      <c r="H125" s="38"/>
+      <c r="I125" s="38"/>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A126" s="39">
+        <v>125</v>
+      </c>
+      <c r="B126" s="38"/>
+      <c r="C126" s="39"/>
+      <c r="D126" s="39"/>
+      <c r="E126" s="39"/>
+      <c r="F126" s="39"/>
+      <c r="G126" s="38"/>
+      <c r="H126" s="38"/>
+      <c r="I126" s="38"/>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A127" s="39">
+        <v>126</v>
+      </c>
+      <c r="B127" s="38"/>
+      <c r="C127" s="39"/>
+      <c r="D127" s="39"/>
+      <c r="E127" s="39"/>
+      <c r="F127" s="39"/>
+      <c r="G127" s="38"/>
+      <c r="H127" s="38"/>
+      <c r="I127" s="38"/>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A128" s="39">
+        <v>127</v>
+      </c>
+      <c r="B128" s="38"/>
+      <c r="C128" s="39"/>
+      <c r="D128" s="39"/>
+      <c r="E128" s="39"/>
+      <c r="F128" s="39"/>
+      <c r="G128" s="38"/>
+      <c r="H128" s="38"/>
+      <c r="I128" s="38"/>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A129" s="39">
+        <v>128</v>
+      </c>
+      <c r="B129" s="38"/>
+      <c r="C129" s="39"/>
+      <c r="D129" s="39"/>
+      <c r="E129" s="39"/>
+      <c r="F129" s="39"/>
+      <c r="G129" s="38"/>
+      <c r="H129" s="38"/>
+      <c r="I129" s="38"/>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A130" s="39">
+        <v>129</v>
+      </c>
+      <c r="B130" s="38"/>
+      <c r="C130" s="39"/>
+      <c r="D130" s="39"/>
+      <c r="E130" s="39"/>
+      <c r="F130" s="39"/>
+      <c r="G130" s="38"/>
+      <c r="H130" s="38"/>
+      <c r="I130" s="38"/>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A131" s="39">
+        <v>130</v>
+      </c>
+      <c r="B131" s="38"/>
+      <c r="C131" s="39"/>
+      <c r="D131" s="39"/>
+      <c r="E131" s="39"/>
+      <c r="F131" s="39"/>
+      <c r="G131" s="38"/>
+      <c r="H131" s="38"/>
+      <c r="I131" s="38"/>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A132" s="39">
+        <v>131</v>
+      </c>
+      <c r="B132" s="38"/>
+      <c r="C132" s="39"/>
+      <c r="D132" s="39"/>
+      <c r="E132" s="39"/>
+      <c r="F132" s="39"/>
+      <c r="G132" s="38"/>
+      <c r="H132" s="38"/>
+      <c r="I132" s="38"/>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A133" s="39">
+        <v>132</v>
+      </c>
+      <c r="B133" s="38"/>
+      <c r="C133" s="39"/>
+      <c r="D133" s="39"/>
+      <c r="E133" s="39"/>
+      <c r="F133" s="39"/>
+      <c r="G133" s="38"/>
+      <c r="H133" s="38"/>
+      <c r="I133" s="38"/>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A134" s="39">
+        <v>133</v>
+      </c>
+      <c r="B134" s="38"/>
+      <c r="C134" s="39"/>
+      <c r="D134" s="39"/>
+      <c r="E134" s="39"/>
+      <c r="F134" s="39"/>
+      <c r="G134" s="38"/>
+      <c r="H134" s="38"/>
+      <c r="I134" s="38"/>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A135" s="39">
+        <v>134</v>
+      </c>
+      <c r="B135" s="38"/>
+      <c r="C135" s="39"/>
+      <c r="D135" s="39"/>
+      <c r="E135" s="39"/>
+      <c r="F135" s="39"/>
+      <c r="G135" s="38"/>
+      <c r="H135" s="38"/>
+      <c r="I135" s="38"/>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A136" s="39">
+        <v>135</v>
+      </c>
+      <c r="B136" s="38"/>
+      <c r="C136" s="39"/>
+      <c r="D136" s="39"/>
+      <c r="E136" s="39"/>
+      <c r="F136" s="39"/>
+      <c r="G136" s="38"/>
+      <c r="H136" s="38"/>
+      <c r="I136" s="38"/>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A137" s="39">
+        <v>136</v>
+      </c>
+      <c r="B137" s="38"/>
+      <c r="C137" s="39"/>
+      <c r="D137" s="39"/>
+      <c r="E137" s="39"/>
+      <c r="F137" s="39"/>
+      <c r="G137" s="38"/>
+      <c r="H137" s="38"/>
+      <c r="I137" s="38"/>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A138" s="39">
+        <v>137</v>
+      </c>
+      <c r="B138" s="38"/>
+      <c r="C138" s="39"/>
+      <c r="D138" s="39"/>
+      <c r="E138" s="39"/>
+      <c r="F138" s="39"/>
+      <c r="G138" s="38"/>
+      <c r="H138" s="38"/>
+      <c r="I138" s="38"/>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A139" s="39">
+        <v>138</v>
+      </c>
+      <c r="B139" s="38"/>
+      <c r="C139" s="39"/>
+      <c r="D139" s="39"/>
+      <c r="E139" s="39"/>
+      <c r="F139" s="39"/>
+      <c r="G139" s="38"/>
+      <c r="H139" s="38"/>
+      <c r="I139" s="38"/>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A140" s="39">
+        <v>139</v>
+      </c>
+      <c r="B140" s="38"/>
+      <c r="C140" s="39"/>
+      <c r="D140" s="39"/>
+      <c r="E140" s="39"/>
+      <c r="F140" s="39"/>
+      <c r="G140" s="38"/>
+      <c r="H140" s="38"/>
+      <c r="I140" s="38"/>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A141" s="39">
+        <v>140</v>
+      </c>
+      <c r="B141" s="38"/>
+      <c r="C141" s="39"/>
+      <c r="D141" s="39"/>
+      <c r="E141" s="39"/>
+      <c r="F141" s="39"/>
+      <c r="G141" s="38"/>
+      <c r="H141" s="38"/>
+      <c r="I141" s="38"/>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A142" s="39">
+        <v>141</v>
+      </c>
+      <c r="B142" s="38"/>
+      <c r="C142" s="39"/>
+      <c r="D142" s="39"/>
+      <c r="E142" s="39"/>
+      <c r="F142" s="39"/>
+      <c r="G142" s="38"/>
+      <c r="H142" s="38"/>
+      <c r="I142" s="38"/>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A143" s="39">
+        <v>142</v>
+      </c>
+      <c r="B143" s="38"/>
+      <c r="C143" s="39"/>
+      <c r="D143" s="39"/>
+      <c r="E143" s="39"/>
+      <c r="F143" s="39"/>
+      <c r="G143" s="38"/>
+      <c r="H143" s="38"/>
+      <c r="I143" s="38"/>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A144" s="39">
+        <v>143</v>
+      </c>
+      <c r="B144" s="38"/>
+      <c r="C144" s="39"/>
+      <c r="D144" s="39"/>
+      <c r="E144" s="39"/>
+      <c r="F144" s="39"/>
+      <c r="G144" s="38"/>
+      <c r="H144" s="38"/>
+      <c r="I144" s="38"/>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A145" s="39">
+        <v>144</v>
+      </c>
+      <c r="B145" s="38"/>
+      <c r="C145" s="39"/>
+      <c r="D145" s="39"/>
+      <c r="E145" s="39"/>
+      <c r="F145" s="39"/>
+      <c r="G145" s="38"/>
+      <c r="H145" s="38"/>
+      <c r="I145" s="38"/>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A146" s="39">
+        <v>145</v>
+      </c>
+      <c r="B146" s="38"/>
+      <c r="C146" s="39"/>
+      <c r="D146" s="39"/>
+      <c r="E146" s="39"/>
+      <c r="F146" s="39"/>
+      <c r="G146" s="38"/>
+      <c r="H146" s="38"/>
+      <c r="I146" s="38"/>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A147" s="39">
+        <v>146</v>
+      </c>
+      <c r="B147" s="38"/>
+      <c r="C147" s="39"/>
+      <c r="D147" s="39"/>
+      <c r="E147" s="39"/>
+      <c r="F147" s="39"/>
+      <c r="G147" s="38"/>
+      <c r="H147" s="38"/>
+      <c r="I147" s="38"/>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A148" s="39">
+        <v>147</v>
+      </c>
+      <c r="B148" s="38"/>
+      <c r="C148" s="39"/>
+      <c r="D148" s="39"/>
+      <c r="E148" s="39"/>
+      <c r="F148" s="39"/>
+      <c r="G148" s="38"/>
+      <c r="H148" s="38"/>
+      <c r="I148" s="38"/>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A149" s="39">
+        <v>148</v>
+      </c>
+      <c r="B149" s="38"/>
+      <c r="C149" s="39"/>
+      <c r="D149" s="39"/>
+      <c r="E149" s="39"/>
+      <c r="F149" s="39"/>
+      <c r="G149" s="38"/>
+      <c r="H149" s="38"/>
+      <c r="I149" s="38"/>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A150" s="39">
+        <v>149</v>
+      </c>
+      <c r="B150" s="38"/>
+      <c r="C150" s="39"/>
+      <c r="D150" s="39"/>
+      <c r="E150" s="39"/>
+      <c r="F150" s="39"/>
+      <c r="G150" s="38"/>
+      <c r="H150" s="38"/>
+      <c r="I150" s="38"/>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A151" s="39">
+        <v>150</v>
+      </c>
+      <c r="B151" s="38"/>
+      <c r="C151" s="39"/>
+      <c r="D151" s="39"/>
+      <c r="E151" s="39"/>
+      <c r="F151" s="39"/>
+      <c r="G151" s="38"/>
+      <c r="H151" s="38"/>
+      <c r="I151" s="38"/>
     </row>
   </sheetData>
   <phoneticPr fontId="13" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{523AED77-7E38-41E9-8D48-E2AD67E3D82E}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{745B6B86-6724-4DD0-9E1F-9F8816721174}"/>
+    <hyperlink ref="H4" r:id="rId3" xr:uid="{B090BCBD-4B93-4787-840D-17A862100EA9}"/>
+    <hyperlink ref="H5" r:id="rId4" xr:uid="{91B52575-65F6-44D5-9A2B-821B36A34197}"/>
+    <hyperlink ref="H6" r:id="rId5" xr:uid="{035CEA30-5611-40F9-BC57-25F99E4512FD}"/>
+    <hyperlink ref="H7" r:id="rId6" xr:uid="{B3E2AA96-FB22-48FD-9E7E-761263DA97B6}"/>
+    <hyperlink ref="H8" r:id="rId7" xr:uid="{2AC69836-6ED8-4511-81D8-1B168A185A15}"/>
+    <hyperlink ref="H9" r:id="rId8" xr:uid="{1B41A758-6415-47ED-B6A2-F944974E0292}"/>
+    <hyperlink ref="H10" r:id="rId9" xr:uid="{D3DFBDB5-C357-4A87-AB47-41F670505585}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Site updated: 2019-02-05 13:18:55
</commit_message>
<xml_diff>
--- a/posts/成长记录/我的2019年目标跟踪记录/目标跟踪表.xlsx
+++ b/posts/成长记录/我的2019年目标跟踪记录/目标跟踪表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\Blog\source\_posts\成长记录\我的2019年目标跟踪记录\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF730592-52A5-48D1-841D-15AD2AF34CD5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127298D7-EA56-4769-B9D9-4AC88EA6B1DF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760" tabRatio="788" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="96">
   <si>
     <t>星期一</t>
   </si>
@@ -471,10 +471,6 @@
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
   <si>
-    <t>设计行为学</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
     <t>如何戒掉坏习惯</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
@@ -624,6 +620,18 @@
   </si>
   <si>
     <t>惊讶心理学</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>设计行为学：打造峰值体验</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://blog.ruanxinyu.cn/posts/%E8%AF%BB%E4%B9%A6%E7%AC%94%E8%AE%B0/%E8%A1%8C%E4%B8%BA%E8%AE%BE%E8%AE%A1%E5%AD%A6-%E6%89%93%E9%80%A0%E5%B3%B0%E5%80%BC%E4%BD%93%E9%AA%8C/</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://blog.ruanxinyu.cn/posts/%E8%AF%BB%E4%B9%A6%E7%AC%94%E8%AE%B0/%E8%B0%81%E8%AF%B4%E4%BD%A0%E4%B8%8D%E8%83%BD%E5%9D%9A%E6%8C%81/</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
 </sst>
@@ -1128,12 +1136,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1152,9 +1154,6 @@
     <xf numFmtId="0" fontId="12" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1171,6 +1170,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1546,10 +1554,10 @@
       <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="38" t="s">
+      <c r="I1" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="38"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="2" t="s">
         <v>43</v>
       </c>
@@ -1575,10 +1583,10 @@
       <c r="H2" s="8">
         <v>43471</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="31"/>
+      <c r="J2" s="43"/>
       <c r="K2" s="17" t="s">
         <v>34</v>
       </c>
@@ -1602,10 +1610,10 @@
         <f>SUM(B3:H3)</f>
         <v>37</v>
       </c>
-      <c r="J3" s="35" t="s">
+      <c r="J3" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="39" t="s">
+      <c r="K3" s="36" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1624,8 +1632,8 @@
         <f t="shared" ref="I4:I67" si="0">SUM(B4:H4)</f>
         <v>0</v>
       </c>
-      <c r="J4" s="36"/>
-      <c r="K4" s="39"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="36"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
@@ -1644,8 +1652,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="J5" s="37"/>
-      <c r="K5" s="39"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="36"/>
     </row>
     <row r="6" spans="1:11" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
@@ -1670,11 +1678,11 @@
       <c r="H6" s="8">
         <v>43478</v>
       </c>
-      <c r="I6" s="31" t="s">
+      <c r="I6" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="31"/>
-      <c r="K6" s="39"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="36"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
@@ -1705,10 +1713,10 @@
         <f t="shared" si="0"/>
         <v>175</v>
       </c>
-      <c r="J7" s="35" t="s">
+      <c r="J7" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="K7" s="39"/>
+      <c r="K7" s="36"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
@@ -1733,8 +1741,8 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="J8" s="36"/>
-      <c r="K8" s="39"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="36"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
@@ -1765,8 +1773,8 @@
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="J9" s="37"/>
-      <c r="K9" s="39"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="36"/>
     </row>
     <row r="10" spans="1:11" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
@@ -1791,11 +1799,11 @@
       <c r="H10" s="8">
         <v>43485</v>
       </c>
-      <c r="I10" s="31" t="s">
+      <c r="I10" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="31"/>
-      <c r="K10" s="39"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="36"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
@@ -1826,10 +1834,10 @@
         <f t="shared" si="0"/>
         <v>149</v>
       </c>
-      <c r="J11" s="35" t="s">
+      <c r="J11" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="K11" s="39"/>
+      <c r="K11" s="36"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
@@ -1852,8 +1860,8 @@
         <f t="shared" si="0"/>
         <v>8.98</v>
       </c>
-      <c r="J12" s="36"/>
-      <c r="K12" s="39"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="36"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
@@ -1878,8 +1886,8 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="J13" s="37"/>
-      <c r="K13" s="39"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="36"/>
     </row>
     <row r="14" spans="1:11" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
@@ -1904,11 +1912,11 @@
       <c r="H14" s="8">
         <v>43492</v>
       </c>
-      <c r="I14" s="31" t="s">
+      <c r="I14" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="J14" s="31"/>
-      <c r="K14" s="39"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="36"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
@@ -1939,10 +1947,10 @@
         <f t="shared" si="0"/>
         <v>201</v>
       </c>
-      <c r="J15" s="35" t="s">
+      <c r="J15" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="K15" s="39"/>
+      <c r="K15" s="36"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
@@ -1967,8 +1975,8 @@
         <f t="shared" si="0"/>
         <v>11.92</v>
       </c>
-      <c r="J16" s="36"/>
-      <c r="K16" s="39"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="36"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
@@ -1999,8 +2007,8 @@
         <f t="shared" si="0"/>
         <v>84</v>
       </c>
-      <c r="J17" s="37"/>
-      <c r="K17" s="39"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="36"/>
     </row>
     <row r="18" spans="1:11" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
@@ -2025,10 +2033,10 @@
       <c r="H18" s="10">
         <v>43499</v>
       </c>
-      <c r="I18" s="30" t="s">
+      <c r="I18" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="J18" s="30"/>
+      <c r="J18" s="44"/>
       <c r="K18" s="18" t="s">
         <v>35</v>
       </c>
@@ -2062,10 +2070,10 @@
         <f t="shared" si="0"/>
         <v>201</v>
       </c>
-      <c r="J19" s="32" t="s">
+      <c r="J19" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="K19" s="40"/>
+      <c r="K19" s="37"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
@@ -2090,8 +2098,8 @@
         <f t="shared" si="0"/>
         <v>13.19</v>
       </c>
-      <c r="J20" s="33"/>
-      <c r="K20" s="41"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="38"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
@@ -2122,8 +2130,8 @@
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="J21" s="34"/>
-      <c r="K21" s="41"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="38"/>
     </row>
     <row r="22" spans="1:11" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A22" s="10"/>
@@ -2148,11 +2156,11 @@
       <c r="H22" s="10">
         <v>43506</v>
       </c>
-      <c r="I22" s="30" t="s">
+      <c r="I22" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J22" s="30"/>
-      <c r="K22" s="41"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="38"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
@@ -2169,8 +2177,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J23" s="32"/>
-      <c r="K23" s="41"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="38"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
@@ -2187,8 +2195,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J24" s="33"/>
-      <c r="K24" s="41"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="38"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
@@ -2205,8 +2213,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J25" s="34"/>
-      <c r="K25" s="41"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="38"/>
     </row>
     <row r="26" spans="1:11" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A26" s="12"/>
@@ -2231,11 +2239,11 @@
       <c r="H26" s="10">
         <v>43513</v>
       </c>
-      <c r="I26" s="30" t="s">
+      <c r="I26" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="J26" s="30"/>
-      <c r="K26" s="41"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="38"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
@@ -2252,8 +2260,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J27" s="32"/>
-      <c r="K27" s="41"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="38"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
@@ -2270,8 +2278,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J28" s="33"/>
-      <c r="K28" s="41"/>
+      <c r="J28" s="31"/>
+      <c r="K28" s="38"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
@@ -2288,8 +2296,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J29" s="34"/>
-      <c r="K29" s="41"/>
+      <c r="J29" s="32"/>
+      <c r="K29" s="38"/>
     </row>
     <row r="30" spans="1:11" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A30" s="12"/>
@@ -2314,11 +2322,11 @@
       <c r="H30" s="10">
         <v>43520</v>
       </c>
-      <c r="I30" s="30" t="s">
+      <c r="I30" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="J30" s="30"/>
-      <c r="K30" s="41"/>
+      <c r="J30" s="44"/>
+      <c r="K30" s="38"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
@@ -2335,8 +2343,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J31" s="32"/>
-      <c r="K31" s="41"/>
+      <c r="J31" s="30"/>
+      <c r="K31" s="38"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
@@ -2353,8 +2361,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J32" s="33"/>
-      <c r="K32" s="41"/>
+      <c r="J32" s="31"/>
+      <c r="K32" s="38"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
@@ -2371,8 +2379,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J33" s="34"/>
-      <c r="K33" s="42"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="39"/>
     </row>
     <row r="34" spans="1:11" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A34" s="12"/>
@@ -2397,10 +2405,10 @@
       <c r="H34" s="8">
         <v>43527</v>
       </c>
-      <c r="I34" s="31" t="s">
+      <c r="I34" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="J34" s="31"/>
+      <c r="J34" s="43"/>
       <c r="K34" s="17" t="s">
         <v>36</v>
       </c>
@@ -2420,8 +2428,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J35" s="35"/>
-      <c r="K35" s="40"/>
+      <c r="J35" s="33"/>
+      <c r="K35" s="37"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
@@ -2438,8 +2446,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J36" s="36"/>
-      <c r="K36" s="41"/>
+      <c r="J36" s="34"/>
+      <c r="K36" s="38"/>
     </row>
     <row r="37" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
@@ -2456,8 +2464,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J37" s="37"/>
-      <c r="K37" s="41"/>
+      <c r="J37" s="35"/>
+      <c r="K37" s="38"/>
     </row>
     <row r="38" spans="1:11" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A38" s="7"/>
@@ -2482,11 +2490,11 @@
       <c r="H38" s="8">
         <v>43534</v>
       </c>
-      <c r="I38" s="31" t="s">
+      <c r="I38" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="J38" s="31"/>
-      <c r="K38" s="41"/>
+      <c r="J38" s="43"/>
+      <c r="K38" s="38"/>
     </row>
     <row r="39" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
@@ -2503,8 +2511,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J39" s="35"/>
-      <c r="K39" s="41"/>
+      <c r="J39" s="33"/>
+      <c r="K39" s="38"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
@@ -2521,8 +2529,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J40" s="36"/>
-      <c r="K40" s="41"/>
+      <c r="J40" s="34"/>
+      <c r="K40" s="38"/>
     </row>
     <row r="41" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
@@ -2539,8 +2547,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J41" s="37"/>
-      <c r="K41" s="41"/>
+      <c r="J41" s="35"/>
+      <c r="K41" s="38"/>
     </row>
     <row r="42" spans="1:11" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A42" s="7"/>
@@ -2565,11 +2573,11 @@
       <c r="H42" s="8">
         <v>43541</v>
       </c>
-      <c r="I42" s="31" t="s">
+      <c r="I42" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="J42" s="31"/>
-      <c r="K42" s="41"/>
+      <c r="J42" s="43"/>
+      <c r="K42" s="38"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
@@ -2586,8 +2594,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J43" s="35"/>
-      <c r="K43" s="41"/>
+      <c r="J43" s="33"/>
+      <c r="K43" s="38"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
@@ -2604,8 +2612,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J44" s="36"/>
-      <c r="K44" s="41"/>
+      <c r="J44" s="34"/>
+      <c r="K44" s="38"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
@@ -2622,8 +2630,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J45" s="37"/>
-      <c r="K45" s="41"/>
+      <c r="J45" s="35"/>
+      <c r="K45" s="38"/>
     </row>
     <row r="46" spans="1:11" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A46" s="7"/>
@@ -2648,11 +2656,11 @@
       <c r="H46" s="8">
         <v>43548</v>
       </c>
-      <c r="I46" s="31" t="s">
+      <c r="I46" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="J46" s="31"/>
-      <c r="K46" s="41"/>
+      <c r="J46" s="43"/>
+      <c r="K46" s="38"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
@@ -2669,8 +2677,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J47" s="35"/>
-      <c r="K47" s="41"/>
+      <c r="J47" s="33"/>
+      <c r="K47" s="38"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
@@ -2687,8 +2695,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J48" s="36"/>
-      <c r="K48" s="41"/>
+      <c r="J48" s="34"/>
+      <c r="K48" s="38"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="9" t="s">
@@ -2705,8 +2713,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J49" s="37"/>
-      <c r="K49" s="41"/>
+      <c r="J49" s="35"/>
+      <c r="K49" s="38"/>
     </row>
     <row r="50" spans="1:11" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A50" s="7"/>
@@ -2731,11 +2739,11 @@
       <c r="H50" s="8">
         <v>43555</v>
       </c>
-      <c r="I50" s="31" t="s">
+      <c r="I50" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="J50" s="31"/>
-      <c r="K50" s="41"/>
+      <c r="J50" s="43"/>
+      <c r="K50" s="38"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="9" t="s">
@@ -2752,8 +2760,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J51" s="35"/>
-      <c r="K51" s="41"/>
+      <c r="J51" s="33"/>
+      <c r="K51" s="38"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
@@ -2770,8 +2778,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J52" s="36"/>
-      <c r="K52" s="41"/>
+      <c r="J52" s="34"/>
+      <c r="K52" s="38"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="9" t="s">
@@ -2788,8 +2796,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J53" s="37"/>
-      <c r="K53" s="42"/>
+      <c r="J53" s="35"/>
+      <c r="K53" s="39"/>
     </row>
     <row r="54" spans="1:11" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A54" s="12"/>
@@ -2814,10 +2822,10 @@
       <c r="H54" s="10">
         <v>43562</v>
       </c>
-      <c r="I54" s="30" t="s">
+      <c r="I54" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="J54" s="30"/>
+      <c r="J54" s="44"/>
       <c r="K54" s="18" t="s">
         <v>37</v>
       </c>
@@ -2837,8 +2845,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J55" s="32"/>
-      <c r="K55" s="40"/>
+      <c r="J55" s="30"/>
+      <c r="K55" s="37"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
@@ -2855,8 +2863,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J56" s="33"/>
-      <c r="K56" s="41"/>
+      <c r="J56" s="31"/>
+      <c r="K56" s="38"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="11" t="s">
@@ -2873,8 +2881,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J57" s="34"/>
-      <c r="K57" s="41"/>
+      <c r="J57" s="32"/>
+      <c r="K57" s="38"/>
     </row>
     <row r="58" spans="1:11" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A58" s="12"/>
@@ -2899,11 +2907,11 @@
       <c r="H58" s="10">
         <v>43569</v>
       </c>
-      <c r="I58" s="30" t="s">
+      <c r="I58" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="J58" s="30"/>
-      <c r="K58" s="41"/>
+      <c r="J58" s="44"/>
+      <c r="K58" s="38"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="11" t="s">
@@ -2920,8 +2928,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J59" s="32"/>
-      <c r="K59" s="41"/>
+      <c r="J59" s="30"/>
+      <c r="K59" s="38"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="11" t="s">
@@ -2938,8 +2946,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J60" s="33"/>
-      <c r="K60" s="41"/>
+      <c r="J60" s="31"/>
+      <c r="K60" s="38"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="11" t="s">
@@ -2956,8 +2964,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J61" s="34"/>
-      <c r="K61" s="41"/>
+      <c r="J61" s="32"/>
+      <c r="K61" s="38"/>
     </row>
     <row r="62" spans="1:11" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A62" s="12"/>
@@ -2982,11 +2990,11 @@
       <c r="H62" s="10">
         <v>43576</v>
       </c>
-      <c r="I62" s="30" t="s">
+      <c r="I62" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="J62" s="30"/>
-      <c r="K62" s="41"/>
+      <c r="J62" s="44"/>
+      <c r="K62" s="38"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="11" t="s">
@@ -3003,8 +3011,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J63" s="32"/>
-      <c r="K63" s="41"/>
+      <c r="J63" s="30"/>
+      <c r="K63" s="38"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="11" t="s">
@@ -3021,8 +3029,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J64" s="33"/>
-      <c r="K64" s="41"/>
+      <c r="J64" s="31"/>
+      <c r="K64" s="38"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="11" t="s">
@@ -3039,8 +3047,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J65" s="34"/>
-      <c r="K65" s="41"/>
+      <c r="J65" s="32"/>
+      <c r="K65" s="38"/>
     </row>
     <row r="66" spans="1:11" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A66" s="12"/>
@@ -3065,11 +3073,11 @@
       <c r="H66" s="10">
         <v>43583</v>
       </c>
-      <c r="I66" s="30" t="s">
+      <c r="I66" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="J66" s="30"/>
-      <c r="K66" s="41"/>
+      <c r="J66" s="44"/>
+      <c r="K66" s="38"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="11" t="s">
@@ -3086,8 +3094,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J67" s="32"/>
-      <c r="K67" s="41"/>
+      <c r="J67" s="30"/>
+      <c r="K67" s="38"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="11" t="s">
@@ -3104,8 +3112,8 @@
         <f t="shared" ref="I68:I73" si="1">SUM(B68:H68)</f>
         <v>0</v>
       </c>
-      <c r="J68" s="33"/>
-      <c r="K68" s="41"/>
+      <c r="J68" s="31"/>
+      <c r="K68" s="38"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="11" t="s">
@@ -3122,8 +3130,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J69" s="34"/>
-      <c r="K69" s="42"/>
+      <c r="J69" s="32"/>
+      <c r="K69" s="39"/>
     </row>
     <row r="70" spans="1:11" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A70" s="12"/>
@@ -3148,10 +3156,10 @@
       <c r="H70" s="8">
         <v>43590</v>
       </c>
-      <c r="I70" s="43" t="s">
+      <c r="I70" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="J70" s="44"/>
+      <c r="J70" s="41"/>
       <c r="K70" s="17" t="s">
         <v>38</v>
       </c>
@@ -3171,8 +3179,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J71" s="35"/>
-      <c r="K71" s="40"/>
+      <c r="J71" s="33"/>
+      <c r="K71" s="37"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="11" t="s">
@@ -3189,8 +3197,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J72" s="36"/>
-      <c r="K72" s="41"/>
+      <c r="J72" s="34"/>
+      <c r="K72" s="38"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="11" t="s">
@@ -3207,8 +3215,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J73" s="37"/>
-      <c r="K73" s="42"/>
+      <c r="J73" s="35"/>
+      <c r="K73" s="39"/>
     </row>
     <row r="1048575" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B1048575" s="1">
@@ -3242,6 +3250,32 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I62:J62"/>
+    <mergeCell ref="I66:J66"/>
+    <mergeCell ref="J63:J65"/>
+    <mergeCell ref="J59:J61"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="J51:J53"/>
+    <mergeCell ref="J55:J57"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="I54:J54"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="J3:J5"/>
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="J11:J13"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I14:J14"/>
     <mergeCell ref="J67:J69"/>
     <mergeCell ref="J71:J73"/>
     <mergeCell ref="K3:K17"/>
@@ -3258,32 +3292,6 @@
     <mergeCell ref="J39:J41"/>
     <mergeCell ref="J43:J45"/>
     <mergeCell ref="J47:J49"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="J3:J5"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="J11:J13"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I62:J62"/>
-    <mergeCell ref="I66:J66"/>
-    <mergeCell ref="J63:J65"/>
-    <mergeCell ref="J59:J61"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="J51:J53"/>
-    <mergeCell ref="J55:J57"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="I54:J54"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="I6:J6"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -3298,7 +3306,7 @@
   <dimension ref="A1:I151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3330,7 +3338,7 @@
         <v>47</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H1" s="22" t="s">
         <v>48</v>
@@ -3357,7 +3365,7 @@
         <v>52</v>
       </c>
       <c r="G2" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H2" s="26" t="s">
         <v>53</v>
@@ -3384,7 +3392,7 @@
         <v>52</v>
       </c>
       <c r="G3" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H3" s="26" t="s">
         <v>55</v>
@@ -3411,7 +3419,7 @@
         <v>52</v>
       </c>
       <c r="G4" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H4" s="26" t="s">
         <v>57</v>
@@ -3438,7 +3446,7 @@
         <v>52</v>
       </c>
       <c r="G5" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H5" s="26" t="s">
         <v>58</v>
@@ -3465,7 +3473,7 @@
         <v>52</v>
       </c>
       <c r="G6" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H6" s="26" t="s">
         <v>60</v>
@@ -3492,7 +3500,7 @@
         <v>52</v>
       </c>
       <c r="G7" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H7" s="26" t="s">
         <v>62</v>
@@ -3519,7 +3527,7 @@
         <v>52</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H8" s="26" t="s">
         <v>64</v>
@@ -3546,7 +3554,7 @@
         <v>52</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H9" s="26" t="s">
         <v>66</v>
@@ -3573,7 +3581,7 @@
         <v>52</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H10" s="26" t="s">
         <v>68</v>
@@ -3585,7 +3593,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C11" s="24" t="s">
         <v>52</v>
@@ -3600,7 +3608,7 @@
         <v>52</v>
       </c>
       <c r="G11" s="27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H11" s="23"/>
       <c r="I11" s="23"/>
@@ -3610,7 +3618,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C12" s="24" t="s">
         <v>52</v>
@@ -3625,7 +3633,7 @@
         <v>52</v>
       </c>
       <c r="G12" s="27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H12" s="23"/>
       <c r="I12" s="23"/>
@@ -3635,7 +3643,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C13" s="24" t="s">
         <v>52</v>
@@ -3650,7 +3658,7 @@
         <v>52</v>
       </c>
       <c r="G13" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H13" s="23"/>
       <c r="I13" s="23"/>
@@ -3671,11 +3679,15 @@
       <c r="E14" s="24">
         <v>3</v>
       </c>
-      <c r="F14" s="24"/>
+      <c r="F14" s="24">
+        <v>2</v>
+      </c>
       <c r="G14" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="H14" s="23"/>
+        <v>74</v>
+      </c>
+      <c r="H14" s="26" t="s">
+        <v>95</v>
+      </c>
       <c r="I14" s="23"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -3683,7 +3695,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="C15" s="29">
         <v>43498</v>
@@ -3694,11 +3706,15 @@
       <c r="E15" s="24">
         <v>4.5</v>
       </c>
-      <c r="F15" s="24"/>
+      <c r="F15" s="24">
+        <v>2.5</v>
+      </c>
       <c r="G15" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="H15" s="23"/>
+        <v>74</v>
+      </c>
+      <c r="H15" s="26" t="s">
+        <v>94</v>
+      </c>
       <c r="I15" s="23"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -3706,18 +3722,18 @@
         <v>15</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C16" s="29">
         <v>43499</v>
       </c>
       <c r="D16" s="29">
-        <v>43500</v>
+        <v>43501</v>
       </c>
       <c r="E16" s="24"/>
       <c r="F16" s="24"/>
       <c r="G16" s="28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H16" s="23"/>
       <c r="I16" s="23"/>
@@ -3727,7 +3743,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C17" s="24"/>
       <c r="D17" s="24"/>
@@ -3742,7 +3758,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C18" s="24"/>
       <c r="D18" s="24"/>
@@ -3757,7 +3773,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C19" s="24"/>
       <c r="D19" s="24"/>
@@ -3772,7 +3788,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C20" s="24"/>
       <c r="D20" s="24"/>
@@ -3787,7 +3803,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C21" s="24"/>
       <c r="D21" s="24"/>
@@ -3802,7 +3818,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C22" s="24"/>
       <c r="D22" s="24"/>
@@ -3817,7 +3833,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C23" s="24"/>
       <c r="D23" s="24"/>
@@ -3832,7 +3848,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C24" s="24"/>
       <c r="D24" s="24"/>
@@ -3847,7 +3863,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C25" s="24"/>
       <c r="D25" s="24"/>
@@ -3862,7 +3878,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C26" s="24"/>
       <c r="D26" s="24"/>
@@ -3877,7 +3893,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C27" s="24"/>
       <c r="D27" s="24"/>
@@ -3892,7 +3908,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C28" s="24"/>
       <c r="D28" s="24"/>
@@ -5513,8 +5529,10 @@
     <hyperlink ref="H8" r:id="rId7" xr:uid="{2AC69836-6ED8-4511-81D8-1B168A185A15}"/>
     <hyperlink ref="H9" r:id="rId8" xr:uid="{1B41A758-6415-47ED-B6A2-F944974E0292}"/>
     <hyperlink ref="H10" r:id="rId9" xr:uid="{D3DFBDB5-C357-4A87-AB47-41F670505585}"/>
+    <hyperlink ref="H15" r:id="rId10" xr:uid="{92DE3606-13D5-464A-B201-0F8055912BE5}"/>
+    <hyperlink ref="H14" r:id="rId11" xr:uid="{24681DDF-6853-4C23-96CD-01C849B069E2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>